<commit_message>
Add threading, and README.md
</commit_message>
<xml_diff>
--- a/professors_fake.xlsx
+++ b/professors_fake.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>first_name</t>
+  </si>
   <si>
     <t>last_name</t>
   </si>
@@ -44,6 +47,9 @@
   </si>
   <si>
     <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
   </si>
   <si>
     <t>Field</t>
@@ -113,26 +119,26 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -436,79 +442,86 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="23.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="43.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="49.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="19.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="23.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="6" width="43.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="5" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="6" width="49.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4">
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="4">
         <v>2020</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="4">
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="4">
         <v>2022</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>14</v>
+      <c r="H2" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>